<commit_message>
Codes of relationship with scales added and working
</commit_message>
<xml_diff>
--- a/psaw/excel/scales.xlsx
+++ b/psaw/excel/scales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\psy-scales-py\psaw\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A33683A-4BC2-4AB7-B07B-E2D5A153A519}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0127FECD-C9C0-4C9A-92C6-9C10B8DEF455}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B8686CA1-67F7-47D5-A5B5-96D69129525C}"/>
   </bookViews>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="179">
   <si>
     <t>Depression</t>
   </si>
@@ -249,9 +249,6 @@
     <t>BDI</t>
   </si>
   <si>
-    <t xml:space="preserve">PHQ-9 </t>
-  </si>
-  <si>
     <t>DPRS-11</t>
   </si>
   <si>
@@ -691,6 +688,18 @@
   </si>
   <si>
     <t>Related (code)</t>
+  </si>
+  <si>
+    <t>7_8</t>
+  </si>
+  <si>
+    <t>6_10</t>
+  </si>
+  <si>
+    <t>PHQ-9</t>
+  </si>
+  <si>
+    <t>1_4</t>
   </si>
 </sst>
 </file>
@@ -871,7 +880,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -900,6 +909,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -931,21 +953,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -956,10 +979,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1262,8 +1281,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="B2:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1297,971 +1316,969 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="20"/>
+      <c r="C6" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="20"/>
+      <c r="C7" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
-      <c r="C6" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="15"/>
-      <c r="C7" s="8" t="s">
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="20"/>
+      <c r="C8" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
-      <c r="C8" s="8" t="s">
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="20"/>
+      <c r="C9" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="22"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="15"/>
-      <c r="C9" s="8" t="s">
+      <c r="E9" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="20"/>
+      <c r="C10" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="15"/>
-      <c r="C10" s="8" t="s">
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="20"/>
+      <c r="C11" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="15"/>
-      <c r="C11" s="8" t="s">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="20"/>
+      <c r="C12" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="15"/>
-      <c r="C12" s="8" t="s">
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="20"/>
+      <c r="C13" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="15"/>
-      <c r="C13" s="8" t="s">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="20"/>
+      <c r="C14" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="15"/>
-      <c r="C14" s="8" t="s">
+      <c r="E14" s="13"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="20"/>
+      <c r="C15" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="23"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="15"/>
-      <c r="C15" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="22"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="15"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="8" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="22"/>
+        <v>43</v>
+      </c>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="15"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="20"/>
+      <c r="C18" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="22"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="15"/>
-      <c r="C18" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="22"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="20"/>
+      <c r="C20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="15"/>
-      <c r="C20" s="8" t="s">
+      <c r="E20" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="20"/>
+      <c r="C21" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E21" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="20"/>
+      <c r="C22" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="20"/>
+      <c r="C23" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="20"/>
+      <c r="C24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="21"/>
+      <c r="C25" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="14">
+        <v>9</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="17"/>
+      <c r="C27" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="14"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="17"/>
+      <c r="C28" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="17"/>
+      <c r="C29" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="17"/>
+      <c r="C30" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="14">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
-      <c r="C21" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="15"/>
-      <c r="C22" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="15"/>
-      <c r="C23" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="22"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="15"/>
-      <c r="C24" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="22"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B25" s="16"/>
-      <c r="C25" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="22"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="24">
-        <v>9</v>
-      </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="12"/>
-      <c r="C27" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="24"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="12"/>
-      <c r="C28" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="24"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B29" s="12"/>
-      <c r="C29" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="24"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="12"/>
-      <c r="C30" s="10" t="s">
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="17"/>
+      <c r="C31" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="24">
-        <v>7</v>
-      </c>
-      <c r="G30" s="21"/>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="12"/>
-      <c r="C31" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="24">
+      <c r="E31" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="12"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="17"/>
+      <c r="C33" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="12"/>
-      <c r="C33" s="10" t="s">
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="17"/>
+      <c r="C34" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="24"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="12"/>
-      <c r="C34" s="10" t="s">
+      <c r="E34" s="14"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="17"/>
+      <c r="C35" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="12"/>
-      <c r="C35" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="24"/>
+      <c r="E35" s="14"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="12"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E36" s="24">
+        <v>60</v>
+      </c>
+      <c r="E36" s="14">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="12"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B38" s="17"/>
+      <c r="C38" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="24"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="12"/>
-      <c r="C38" s="10" t="s">
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B39" s="17"/>
+      <c r="C39" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="12"/>
-      <c r="C39" s="10" t="s">
+      <c r="E39" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B40" s="17"/>
+      <c r="C40" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B40" s="12"/>
-      <c r="C40" s="10" t="s">
+      <c r="E40" s="14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B41" s="17"/>
+      <c r="C41" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D41" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B41" s="12"/>
-      <c r="C41" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" s="24">
+      <c r="E41" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B42" s="12"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D42" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="14"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="17"/>
+      <c r="C43" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" s="9"/>
+      <c r="E43" s="14"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="17"/>
+      <c r="C44" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="24"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B43" s="12"/>
-      <c r="C43" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="24"/>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B44" s="12"/>
-      <c r="C44" s="10" t="s">
+      <c r="E44" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="18"/>
+      <c r="C45" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B45" s="13"/>
-      <c r="C45" s="9" t="s">
-        <v>137</v>
-      </c>
       <c r="D45" s="9"/>
-      <c r="E45" s="24"/>
+      <c r="E45" s="14"/>
     </row>
     <row r="46" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B46" s="18" t="s">
-        <v>28</v>
+      <c r="B46" s="23" t="s">
+        <v>177</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B47" s="24"/>
+      <c r="C47" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E46" s="22"/>
-    </row>
-    <row r="47" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B47" s="19"/>
-      <c r="C47" s="6" t="s">
+      <c r="E47" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B48" s="24"/>
+      <c r="C48" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D48" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="24"/>
+      <c r="C49" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E47" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B48" s="19"/>
-      <c r="C48" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E48" s="22">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B49" s="19"/>
-      <c r="C49" s="6" t="s">
+      <c r="E49" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="24"/>
+      <c r="C50" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B50" s="19"/>
-      <c r="C50" s="6" t="s">
+      <c r="E50" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B51" s="24"/>
+      <c r="C51" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D51" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E50" s="22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B51" s="19"/>
-      <c r="C51" s="6" t="s">
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="24"/>
+      <c r="C52" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D52" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E51" s="22"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="19"/>
-      <c r="C52" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E52" s="22">
+      <c r="E52" s="12">
         <v>12</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="19"/>
+      <c r="B53" s="24"/>
       <c r="C53" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="7"/>
-      <c r="E53" s="22"/>
+      <c r="E53" s="12"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="19"/>
+      <c r="B54" s="24"/>
       <c r="C54" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="25"/>
+      <c r="C55" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="7"/>
-      <c r="E54" s="22"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="20"/>
-      <c r="C55" s="6" t="s">
+      <c r="D55" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="6" t="s">
+      <c r="D56" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="22">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E56" s="24">
+      <c r="E56" s="14">
         <v>11</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="12"/>
+      <c r="B57" s="17"/>
       <c r="C57" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" s="14"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="17"/>
+      <c r="C58" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D58" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E57" s="24"/>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="12"/>
-      <c r="C58" s="10" t="s">
+      <c r="E58" s="14"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="17"/>
+      <c r="C59" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D59" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E58" s="24"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="12"/>
-      <c r="C59" s="10" t="s">
+      <c r="E59" s="14"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="17"/>
+      <c r="C60" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D60" s="9"/>
+      <c r="E60" s="14"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="17"/>
+      <c r="C61" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D61" s="9"/>
+      <c r="E61" s="14"/>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="17"/>
+      <c r="C62" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E59" s="24"/>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="12"/>
-      <c r="C60" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D60" s="9"/>
-      <c r="E60" s="24"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="12"/>
-      <c r="C61" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D61" s="9"/>
-      <c r="E61" s="24"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="12"/>
-      <c r="C62" s="10" t="s">
+      <c r="E62" s="14"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="17"/>
+      <c r="C63" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D63" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E62" s="24"/>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="12"/>
-      <c r="C63" s="10" t="s">
+      <c r="E63" s="14"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" s="17"/>
+      <c r="C64" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D64" s="9"/>
+      <c r="E64" s="14"/>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="17"/>
+      <c r="C65" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="D65" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E63" s="24"/>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B64" s="12"/>
-      <c r="C64" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="D64" s="9"/>
-      <c r="E64" s="24"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B65" s="12"/>
-      <c r="C65" s="10" t="s">
+      <c r="E65" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="17"/>
+      <c r="C66" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D65" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E65" s="24">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B66" s="12"/>
-      <c r="C66" s="9" t="s">
-        <v>155</v>
-      </c>
       <c r="D66" s="9"/>
-      <c r="E66" s="24"/>
+      <c r="E66" s="14"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B67" s="12"/>
+      <c r="B67" s="17"/>
       <c r="C67" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D67" s="9"/>
-      <c r="E67" s="24"/>
+      <c r="E67" s="14"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B68" s="12"/>
+      <c r="B68" s="17"/>
       <c r="C68" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D68" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E68" s="24"/>
+        <v>82</v>
+      </c>
+      <c r="E68" s="14"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B69" s="12"/>
+      <c r="B69" s="17"/>
       <c r="C69" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D69" s="9"/>
-      <c r="E69" s="24"/>
+      <c r="E69" s="14"/>
     </row>
     <row r="70" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B70" s="12"/>
+      <c r="B70" s="17"/>
       <c r="C70" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E70" s="14"/>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" s="17"/>
+      <c r="C71" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E70" s="24"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B71" s="12"/>
-      <c r="C71" s="9" t="s">
-        <v>158</v>
-      </c>
       <c r="D71" s="9"/>
-      <c r="E71" s="24"/>
+      <c r="E71" s="14"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B72" s="12"/>
+      <c r="B72" s="17"/>
       <c r="C72" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D72" s="9"/>
-      <c r="E72" s="24"/>
+      <c r="E72" s="14"/>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B73" s="12"/>
+      <c r="B73" s="17"/>
       <c r="C73" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D73" s="9"/>
-      <c r="E73" s="24"/>
+      <c r="E73" s="14"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B74" s="12"/>
+      <c r="B74" s="17"/>
       <c r="C74" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E74" s="24">
+        <v>84</v>
+      </c>
+      <c r="E74" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="75" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B75" s="13"/>
+      <c r="B75" s="18"/>
       <c r="C75" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D75" s="9"/>
-      <c r="E75" s="24"/>
+      <c r="E75" s="14"/>
     </row>
     <row r="76" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B76" s="14" t="s">
-        <v>30</v>
+      <c r="B76" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E76" s="22">
+        <v>85</v>
+      </c>
+      <c r="E76" s="12">
         <v>7</v>
       </c>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B77" s="15"/>
+      <c r="B77" s="20"/>
       <c r="C77" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E77" s="22">
+        <v>86</v>
+      </c>
+      <c r="E77" s="12">
         <v>11</v>
       </c>
     </row>
     <row r="78" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B78" s="15"/>
+      <c r="B78" s="20"/>
       <c r="C78" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D78" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E78" s="12"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="20"/>
+      <c r="C79" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D79" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E78" s="22"/>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B79" s="15"/>
-      <c r="C79" s="8" t="s">
+      <c r="E79" s="12"/>
+    </row>
+    <row r="80" spans="2:5" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="20"/>
+      <c r="C80" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="D79" s="8" t="s">
+      <c r="D80" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E79" s="22"/>
-    </row>
-    <row r="80" spans="2:5" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="15"/>
-      <c r="C80" s="8" t="s">
+      <c r="E80" s="12"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B81" s="20"/>
+      <c r="C81" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="D80" s="8" t="s">
+      <c r="D81" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E80" s="22"/>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B81" s="15"/>
-      <c r="C81" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E81" s="22">
+      <c r="E81" s="12">
         <v>2</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B82" s="15"/>
+      <c r="B82" s="20"/>
       <c r="C82" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D82" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E82" s="12"/>
+    </row>
+    <row r="83" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B83" s="20"/>
+      <c r="C83" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E82" s="22"/>
-    </row>
-    <row r="83" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B83" s="15"/>
-      <c r="C83" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E83" s="22"/>
+      <c r="E83" s="12"/>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B84" s="15"/>
+      <c r="B84" s="20"/>
       <c r="C84" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E84" s="22"/>
+        <v>93</v>
+      </c>
+      <c r="E84" s="12"/>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B85" s="16"/>
+      <c r="B85" s="21"/>
       <c r="C85" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D85" s="9"/>
-      <c r="E85" s="22"/>
+      <c r="E85" s="12"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B86" s="17" t="s">
-        <v>29</v>
+      <c r="B86" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="C86" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E86" s="14"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B87" s="22"/>
+      <c r="C87" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="D86" s="10" t="s">
+      <c r="D87" s="9"/>
+      <c r="E87" s="14"/>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B88" s="22"/>
+      <c r="C88" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D88" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E86" s="24"/>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B87" s="17"/>
-      <c r="C87" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D87" s="9"/>
-      <c r="E87" s="24"/>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B88" s="17"/>
-      <c r="C88" s="10" t="s">
+      <c r="E88" s="14"/>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B89" s="22"/>
+      <c r="C89" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="D88" s="10" t="s">
+      <c r="D89" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E88" s="24"/>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B89" s="17"/>
-      <c r="C89" s="10" t="s">
+      <c r="E89" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B90" s="22"/>
+      <c r="C90" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="D89" s="10" t="s">
+      <c r="D90" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B90" s="17"/>
-      <c r="C90" s="10" t="s">
+      <c r="E90" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B91" s="22"/>
+      <c r="C91" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E91" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B92" s="22"/>
+      <c r="C92" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D90" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="E90" s="24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B91" s="17"/>
-      <c r="C91" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D91" s="10" t="s">
+      <c r="D92" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E91" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B92" s="17"/>
-      <c r="C92" s="10" t="s">
+      <c r="E92" s="14"/>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="22"/>
+      <c r="C93" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="D93" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E92" s="24"/>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B93" s="17"/>
-      <c r="C93" s="10" t="s">
+      <c r="E93" s="14"/>
+    </row>
+    <row r="94" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B94" s="22"/>
+      <c r="C94" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="D93" s="10" t="s">
+      <c r="D94" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E93" s="24"/>
-    </row>
-    <row r="94" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B94" s="17"/>
-      <c r="C94" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="D94" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E94" s="24">
+      <c r="E94" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B95" s="17"/>
+      <c r="B95" s="22"/>
       <c r="C95" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D95" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E95" s="24">
-        <v>6.1</v>
+        <v>74</v>
+      </c>
+      <c r="E95" s="14" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B96" s="17"/>
+      <c r="B96" s="22"/>
       <c r="C96" s="10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D96" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="E96" s="24">
+        <v>102</v>
+      </c>
+      <c r="E96" s="14">
         <v>9</v>
       </c>
     </row>
@@ -2274,6 +2291,9 @@
     <mergeCell ref="B26:B45"/>
     <mergeCell ref="B46:B55"/>
   </mergeCells>
+  <conditionalFormatting sqref="E5:E96">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>